<commit_message>
Aggiustata clenaing routine e corretto encoding dei dati
</commit_message>
<xml_diff>
--- a/data/download/Competences-Map-Dataset.xlsx
+++ b/data/download/Competences-Map-Dataset.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="520">
   <si>
     <t>Skills</t>
   </si>
@@ -161,7 +161,7 @@
     <t>Social media strategy</t>
   </si>
   <si>
-    <t>Video production</t>
+    <t>Video Production</t>
   </si>
   <si>
     <t>Advocacy management</t>
@@ -482,9 +482,6 @@
     <t>Interactive Installations</t>
   </si>
   <si>
-    <t>Video Production</t>
-  </si>
-  <si>
     <t>Winemaking expertise</t>
   </si>
   <si>
@@ -818,7 +815,7 @@
     <t>["Multi - Multimedia Museum", "Cultural Avatars", "No Food Tomorrow - Eucarestia", "MODAS: Sas Boghes da sos Singers a Tenor"]</t>
   </si>
   <si>
-    <t>["Multi - Multimedia Museum", "A soup to remember", "TRACTION Opera co-creation for a social transformation", "Weaving Time", "Piccolo Museo del Diario"]</t>
+    <t>["Multi - Multimedia Museum", "ADLaM", "A soup to remember", "TRACTION Opera co-creation for a social transformation", "Weaving Time", "Piccolo Museo del Diario"]</t>
   </si>
   <si>
     <t>["Multi - Multimedia Museum", "Hundred Days: Winemaking Simulator", "Virtual Dance Museum", "Whispering table", "Synthetic Memories", "Craftal", "MEMEX. MEMories and EXperiences for inclusive digital storytelling", "Quantum Temple Path to Alango", "Quantum Temple Passport"]</t>
@@ -1097,6 +1094,12 @@
     <t>["Quantum Temple Path to Alango", "Quantum Temple Passport"]</t>
   </si>
   <si>
+    <t>["HKMALA - Hong Kong Martial Arts Living Archive"]</t>
+  </si>
+  <si>
+    <t>["Multi - Multimedia Museum", "ADLaM", "A soup to remember", "Pub Museums", "THE GREAT PALERMO", "No Food Tomorrow - Eucarestia", "MODAS: Sas Boghes da sos Singers a Tenor", "Camino Al Mictlan NFT", "Whispering table", "History Blocks", "Polifonia Portal", "TRACTION Opera co-creation for a social transformation", "Paderpedia", "Omni ChangâAn Site Concept Show", "Tempio del Brunello", "Renai Dance Animation", "ReCollection", "Synthetic Memories", "Lisbon Under Stars", "Craftal", "Bamboo Weaving Mold", "Urban Media Archive, [unarchiving] program", "Swapmuseun", "ComuniterrÃ e", "Tacit Dialogues", "Cyberknitics", "Kaarigari", "La Baguette stamp", "Fabric Museum: TextLoom", "Weaving Time", "Design philology", "MEMEX. MEMories and EXperiences for inclusive digital storytelling", "RÃ©veil des Archives sonores", "The Living Museum", "Planet Word: The First Voice-Activated Museum", "Piccolo Museo del Diario", "Quantum Temple Path to Alango", "Quantum Temple Passport", "HKMALA - Hong Kong Martial Arts Living Archive", ""]</t>
+  </si>
+  <si>
     <t>projects</t>
   </si>
   <si>
@@ -1112,6 +1115,9 @@
     <t>Multi - Multimedia Museum</t>
   </si>
   <si>
+    <t>Hundred Days: Winemaking Simulator</t>
+  </si>
+  <si>
     <t>ADLaM</t>
   </si>
   <si>
@@ -1121,6 +1127,9 @@
     <t>Pub Museums</t>
   </si>
   <si>
+    <t>THE GREAT PALERMO</t>
+  </si>
+  <si>
     <t>Cultural Avatars</t>
   </si>
   <si>
@@ -1142,6 +1151,9 @@
     <t>MODAS: Sas Boghes da sos Singers a Tenor</t>
   </si>
   <si>
+    <t>Camino Al Mictlan NFT</t>
+  </si>
+  <si>
     <t>Whispering table</t>
   </si>
   <si>
@@ -1160,9 +1172,15 @@
     <t>Paderpedia</t>
   </si>
   <si>
+    <t>Omni ChangâAn Site Concept Show</t>
+  </si>
+  <si>
     <t>Tempio del Brunello</t>
   </si>
   <si>
+    <t>Renai Dance Animation</t>
+  </si>
+  <si>
     <t>ReCollection</t>
   </si>
   <si>
@@ -1175,9 +1193,18 @@
     <t>Craftal</t>
   </si>
   <si>
+    <t>RISE UP - Revitalising Languages and Safeguarding Cultural Diversity</t>
+  </si>
+  <si>
     <t>Bamboo Weaving Mold</t>
   </si>
   <si>
+    <t>Urban Media Archive, [unarchiving] program</t>
+  </si>
+  <si>
+    <t>Swapmuseun</t>
+  </si>
+  <si>
     <t>ComuniterrÃ e</t>
   </si>
   <si>
@@ -1286,6 +1313,9 @@
     <t>["CAD software"]</t>
   </si>
   <si>
+    <t>["Text editing software","Video recording","2D image acquisition technologies"]</t>
+  </si>
+  <si>
     <t>["Audio recording","Motion detection systems","Video recording"]</t>
   </si>
   <si>
@@ -1319,6 +1349,9 @@
     <t>["Storytelling tools","Digital database"]</t>
   </si>
   <si>
+    <t>["Game engine","Simulation algorithms"]</t>
+  </si>
+  <si>
     <t>["Typeface modeling software","Vector graphic software","Text editing software"]</t>
   </si>
   <si>
@@ -1328,6 +1361,9 @@
     <t>["3D modeling software","Augmented Reality (AR)"]</t>
   </si>
   <si>
+    <t>["Visual-novel game engine","Vector graphic software"]</t>
+  </si>
+  <si>
     <t>["Game engine","3D modeling software"]</t>
   </si>
   <si>
@@ -1349,6 +1385,9 @@
     <t>["Audio processing technologies"]</t>
   </si>
   <si>
+    <t>["3D modeling software"]</t>
+  </si>
+  <si>
     <t>["Audio processing technologies","Multimedia development engines"]</t>
   </si>
   <si>
@@ -1367,6 +1406,9 @@
     <t>["Database technologies","Archival systems"]</t>
   </si>
   <si>
+    <t>["Visual Effects software","3D animation software","Digital embroidery tool","3D modeling software","Rendering software"]</t>
+  </si>
+  <si>
     <t>["Machine Learning","Text-to-Image model","NLP - Natural Language Processing"]</t>
   </si>
   <si>
@@ -1424,6 +1466,9 @@
     <t>["Web platform"]</t>
   </si>
   <si>
+    <t>["Game engine","Voice, video, and text communication app"]</t>
+  </si>
+  <si>
     <t>["Cloud Technologies"]</t>
   </si>
   <si>
@@ -1433,6 +1478,9 @@
     <t>["Mobile App","AR technologies"]</t>
   </si>
   <si>
+    <t>["Visual-novel game engine","Web platform"]</t>
+  </si>
+  <si>
     <t>["Game engine","Cloud Technologies"]</t>
   </si>
   <si>
@@ -1451,6 +1499,9 @@
     <t>["Audio streaming platforms"]</t>
   </si>
   <si>
+    <t>["VR","Web3 technologies","Blockchain and NFT technologies"]</t>
+  </si>
+  <si>
     <t>["Sensors","Microcontroller","Motion-activated system","Microphones","Wireless technologies"]</t>
   </si>
   <si>
@@ -1466,9 +1517,15 @@
     <t>["Web platform","Wiki-based platform"]</t>
   </si>
   <si>
+    <t>["Kinetic technologies","Projection mapping technologies"]</t>
+  </si>
+  <si>
     <t>["Mobile App","NFC (Near Field Communication)","Virtual Reality (VR)","Interactive Displays","Projection Mapping technologies","Sensors","Augmented Reality (AR)"]</t>
   </si>
   <si>
+    <t>["Videomaking software","Narrative development software"]</t>
+  </si>
+  <si>
     <t>["Projection mapping technologies","Generative AI","Voice-activated system"]</t>
   </si>
   <si>
@@ -1476,6 +1533,9 @@
   </si>
   <si>
     <t>["Paper printing"]</t>
+  </si>
+  <si>
+    <t>["Media technologies","Social Media"]</t>
   </si>
   <si>
     <t>["Motion Graphic Software","3D printing"]</t>
@@ -1894,10 +1954,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1908,7 +1968,7 @@
         <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1916,10 +1976,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1930,7 +1990,7 @@
         <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1938,10 +1998,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1949,10 +2009,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1960,10 +2020,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1971,10 +2031,10 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1982,10 +2042,10 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1993,10 +2053,10 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C11" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -2004,10 +2064,10 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C12" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -2015,10 +2075,10 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C13" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -2026,10 +2086,10 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2037,10 +2097,10 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C15" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -2048,10 +2108,10 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C16" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -2059,10 +2119,10 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C17" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2070,10 +2130,10 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C18" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2081,10 +2141,10 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C19" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -2092,10 +2152,10 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C20" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -2103,10 +2163,10 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C21" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -2114,10 +2174,10 @@
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C22" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -2125,10 +2185,10 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C23" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -2136,7 +2196,7 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C24" t="s">
         <v>273</v>
@@ -2147,7 +2207,7 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C25" t="s">
         <v>274</v>
@@ -2158,7 +2218,7 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C26" t="s">
         <v>275</v>
@@ -2169,10 +2229,10 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C27" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -2180,10 +2240,10 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C28" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -2191,10 +2251,10 @@
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C29" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -2205,7 +2265,7 @@
         <v>46</v>
       </c>
       <c r="C30" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -2216,7 +2276,7 @@
         <v>46</v>
       </c>
       <c r="C31" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -2224,10 +2284,10 @@
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C32" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -2235,10 +2295,10 @@
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C33" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -2246,7 +2306,7 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C34" t="s">
         <v>279</v>
@@ -2257,7 +2317,7 @@
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C35" t="s">
         <v>280</v>
@@ -2268,10 +2328,10 @@
         <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C36" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -2279,10 +2339,10 @@
         <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C37" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -2290,7 +2350,7 @@
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C38" t="s">
         <v>282</v>
@@ -2301,10 +2361,10 @@
         <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C39" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -2312,10 +2372,10 @@
         <v>41</v>
       </c>
       <c r="B40" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C40" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -2323,7 +2383,7 @@
         <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C41" t="s">
         <v>284</v>
@@ -2334,10 +2394,10 @@
         <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C42" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -2345,10 +2405,10 @@
         <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C43" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -2356,10 +2416,10 @@
         <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C44" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -2370,7 +2430,7 @@
         <v>46</v>
       </c>
       <c r="C45" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -2378,10 +2438,10 @@
         <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C46" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -2389,7 +2449,7 @@
         <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C47" t="s">
         <v>287</v>
@@ -2400,10 +2460,10 @@
         <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C48" t="s">
-        <v>279</v>
+        <v>288</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -2411,10 +2471,10 @@
         <v>50</v>
       </c>
       <c r="B49" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C49" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -2422,10 +2482,10 @@
         <v>51</v>
       </c>
       <c r="B50" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C50" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -2433,7 +2493,7 @@
         <v>52</v>
       </c>
       <c r="B51" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C51" t="s">
         <v>290</v>
@@ -2444,10 +2504,10 @@
         <v>53</v>
       </c>
       <c r="B52" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C52" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -2455,10 +2515,10 @@
         <v>54</v>
       </c>
       <c r="B53" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C53" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -2466,10 +2526,10 @@
         <v>55</v>
       </c>
       <c r="B54" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C54" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -2477,10 +2537,10 @@
         <v>56</v>
       </c>
       <c r="B55" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C55" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -2488,10 +2548,10 @@
         <v>57</v>
       </c>
       <c r="B56" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C56" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -2499,10 +2559,10 @@
         <v>58</v>
       </c>
       <c r="B57" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C57" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -2510,10 +2570,10 @@
         <v>59</v>
       </c>
       <c r="B58" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C58" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -2521,10 +2581,10 @@
         <v>60</v>
       </c>
       <c r="B59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C59" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -2532,10 +2592,10 @@
         <v>61</v>
       </c>
       <c r="B60" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C60" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -2543,10 +2603,10 @@
         <v>62</v>
       </c>
       <c r="B61" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C61" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -2554,7 +2614,7 @@
         <v>63</v>
       </c>
       <c r="B62" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C62" t="s">
         <v>297</v>
@@ -2565,7 +2625,7 @@
         <v>64</v>
       </c>
       <c r="B63" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C63" t="s">
         <v>298</v>
@@ -2576,10 +2636,10 @@
         <v>65</v>
       </c>
       <c r="B64" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C64" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -2587,7 +2647,7 @@
         <v>66</v>
       </c>
       <c r="B65" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C65" t="s">
         <v>299</v>
@@ -2598,10 +2658,10 @@
         <v>67</v>
       </c>
       <c r="B66" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C66" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -2609,7 +2669,7 @@
         <v>68</v>
       </c>
       <c r="B67" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C67" t="s">
         <v>300</v>
@@ -2620,10 +2680,10 @@
         <v>69</v>
       </c>
       <c r="B68" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C68" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -2631,10 +2691,10 @@
         <v>70</v>
       </c>
       <c r="B69" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C69" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -2642,10 +2702,10 @@
         <v>71</v>
       </c>
       <c r="B70" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C70" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -2653,10 +2713,10 @@
         <v>72</v>
       </c>
       <c r="B71" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C71" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -2664,10 +2724,10 @@
         <v>73</v>
       </c>
       <c r="B72" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C72" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -2675,10 +2735,10 @@
         <v>74</v>
       </c>
       <c r="B73" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C73" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -2686,10 +2746,10 @@
         <v>75</v>
       </c>
       <c r="B74" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C74" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -2697,10 +2757,10 @@
         <v>76</v>
       </c>
       <c r="B75" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C75" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -2708,10 +2768,10 @@
         <v>77</v>
       </c>
       <c r="B76" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C76" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -2719,10 +2779,10 @@
         <v>78</v>
       </c>
       <c r="B77" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C77" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -2730,10 +2790,10 @@
         <v>79</v>
       </c>
       <c r="B78" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C78" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -2741,10 +2801,10 @@
         <v>80</v>
       </c>
       <c r="B79" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C79" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -2752,10 +2812,10 @@
         <v>81</v>
       </c>
       <c r="B80" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C80" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -2763,10 +2823,10 @@
         <v>82</v>
       </c>
       <c r="B81" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C81" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -2774,10 +2834,10 @@
         <v>83</v>
       </c>
       <c r="B82" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C82" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -2785,10 +2845,10 @@
         <v>84</v>
       </c>
       <c r="B83" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C83" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -2796,10 +2856,10 @@
         <v>85</v>
       </c>
       <c r="B84" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C84" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -2807,7 +2867,7 @@
         <v>86</v>
       </c>
       <c r="B85" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C85" t="s">
         <v>309</v>
@@ -2818,10 +2878,10 @@
         <v>87</v>
       </c>
       <c r="B86" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C86" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -2829,10 +2889,10 @@
         <v>88</v>
       </c>
       <c r="B87" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C87" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -2840,10 +2900,10 @@
         <v>89</v>
       </c>
       <c r="B88" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C88" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -2851,10 +2911,10 @@
         <v>90</v>
       </c>
       <c r="B89" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C89" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -2862,10 +2922,10 @@
         <v>91</v>
       </c>
       <c r="B90" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C90" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -2873,10 +2933,10 @@
         <v>92</v>
       </c>
       <c r="B91" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C91" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -2884,10 +2944,10 @@
         <v>93</v>
       </c>
       <c r="B92" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C92" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -2895,10 +2955,10 @@
         <v>94</v>
       </c>
       <c r="B93" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C93" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -2906,10 +2966,10 @@
         <v>95</v>
       </c>
       <c r="B94" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C94" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -2917,10 +2977,10 @@
         <v>96</v>
       </c>
       <c r="B95" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C95" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -2928,10 +2988,10 @@
         <v>97</v>
       </c>
       <c r="B96" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C96" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -2939,10 +2999,10 @@
         <v>98</v>
       </c>
       <c r="B97" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C97" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -2950,10 +3010,10 @@
         <v>99</v>
       </c>
       <c r="B98" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C98" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -2961,7 +3021,7 @@
         <v>100</v>
       </c>
       <c r="B99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C99" t="s">
         <v>313</v>
@@ -2972,10 +3032,10 @@
         <v>101</v>
       </c>
       <c r="B100" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C100" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -2983,7 +3043,7 @@
         <v>102</v>
       </c>
       <c r="B101" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C101" t="s">
         <v>314</v>
@@ -2994,10 +3054,10 @@
         <v>103</v>
       </c>
       <c r="B102" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C102" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -3005,10 +3065,10 @@
         <v>104</v>
       </c>
       <c r="B103" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C103" t="s">
-        <v>287</v>
+        <v>316</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -3016,10 +3076,10 @@
         <v>105</v>
       </c>
       <c r="B104" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C104" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -3027,7 +3087,7 @@
         <v>106</v>
       </c>
       <c r="B105" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C105" t="s">
         <v>316</v>
@@ -3038,10 +3098,10 @@
         <v>107</v>
       </c>
       <c r="B106" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C106" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -3049,7 +3109,7 @@
         <v>108</v>
       </c>
       <c r="B107" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C107" t="s">
         <v>318</v>
@@ -3060,10 +3120,10 @@
         <v>109</v>
       </c>
       <c r="B108" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C108" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -3071,10 +3131,10 @@
         <v>110</v>
       </c>
       <c r="B109" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C109" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -3082,10 +3142,10 @@
         <v>111</v>
       </c>
       <c r="B110" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C110" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -3093,10 +3153,10 @@
         <v>112</v>
       </c>
       <c r="B111" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C111" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -3104,10 +3164,10 @@
         <v>113</v>
       </c>
       <c r="B112" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C112" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -3115,10 +3175,10 @@
         <v>114</v>
       </c>
       <c r="B113" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C113" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -3126,10 +3186,10 @@
         <v>115</v>
       </c>
       <c r="B114" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C114" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -3137,10 +3197,10 @@
         <v>116</v>
       </c>
       <c r="B115" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C115" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -3148,10 +3208,10 @@
         <v>117</v>
       </c>
       <c r="B116" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C116" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -3159,10 +3219,10 @@
         <v>118</v>
       </c>
       <c r="B117" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C117" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -3170,10 +3230,10 @@
         <v>119</v>
       </c>
       <c r="B118" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C118" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -3181,10 +3241,10 @@
         <v>120</v>
       </c>
       <c r="B119" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C119" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -3192,10 +3252,10 @@
         <v>121</v>
       </c>
       <c r="B120" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C120" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -3203,10 +3263,10 @@
         <v>122</v>
       </c>
       <c r="B121" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C121" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -3214,7 +3274,7 @@
         <v>123</v>
       </c>
       <c r="B122" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C122" t="s">
         <v>320</v>
@@ -3225,10 +3285,10 @@
         <v>124</v>
       </c>
       <c r="B123" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C123" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -3236,10 +3296,10 @@
         <v>125</v>
       </c>
       <c r="B124" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C124" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -3247,10 +3307,10 @@
         <v>126</v>
       </c>
       <c r="B125" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C125" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -3258,10 +3318,10 @@
         <v>127</v>
       </c>
       <c r="B126" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C126" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -3269,7 +3329,7 @@
         <v>128</v>
       </c>
       <c r="B127" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C127" t="s">
         <v>323</v>
@@ -3280,10 +3340,10 @@
         <v>129</v>
       </c>
       <c r="B128" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C128" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -3291,7 +3351,7 @@
         <v>130</v>
       </c>
       <c r="B129" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C129" t="s">
         <v>324</v>
@@ -3302,7 +3362,7 @@
         <v>131</v>
       </c>
       <c r="B130" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C130" t="s">
         <v>324</v>
@@ -3313,10 +3373,10 @@
         <v>132</v>
       </c>
       <c r="B131" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C131" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -3324,10 +3384,10 @@
         <v>133</v>
       </c>
       <c r="B132" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C132" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -3335,10 +3395,10 @@
         <v>134</v>
       </c>
       <c r="B133" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C133" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -3346,7 +3406,7 @@
         <v>135</v>
       </c>
       <c r="B134" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C134" t="s">
         <v>325</v>
@@ -3357,7 +3417,7 @@
         <v>136</v>
       </c>
       <c r="B135" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C135" t="s">
         <v>325</v>
@@ -3368,7 +3428,7 @@
         <v>137</v>
       </c>
       <c r="B136" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C136" t="s">
         <v>325</v>
@@ -3379,10 +3439,10 @@
         <v>138</v>
       </c>
       <c r="B137" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C137" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -3390,10 +3450,10 @@
         <v>139</v>
       </c>
       <c r="B138" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C138" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -3401,7 +3461,7 @@
         <v>140</v>
       </c>
       <c r="B139" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C139" t="s">
         <v>326</v>
@@ -3412,10 +3472,10 @@
         <v>141</v>
       </c>
       <c r="B140" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C140" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -3423,10 +3483,10 @@
         <v>142</v>
       </c>
       <c r="B141" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C141" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -3434,7 +3494,7 @@
         <v>143</v>
       </c>
       <c r="B142" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C142" t="s">
         <v>327</v>
@@ -3448,7 +3508,7 @@
         <v>46</v>
       </c>
       <c r="C143" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="144" spans="1:3">
@@ -3456,10 +3516,10 @@
         <v>145</v>
       </c>
       <c r="B144" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C144" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -3467,10 +3527,10 @@
         <v>146</v>
       </c>
       <c r="B145" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C145" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -3481,7 +3541,7 @@
         <v>46</v>
       </c>
       <c r="C146" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -3489,7 +3549,7 @@
         <v>148</v>
       </c>
       <c r="B147" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C147" t="s">
         <v>328</v>
@@ -3500,10 +3560,10 @@
         <v>149</v>
       </c>
       <c r="B148" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C148" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -3511,10 +3571,10 @@
         <v>150</v>
       </c>
       <c r="B149" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C149" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -3522,7 +3582,7 @@
         <v>151</v>
       </c>
       <c r="B150" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C150" t="s">
         <v>329</v>
@@ -3533,10 +3593,10 @@
         <v>152</v>
       </c>
       <c r="B151" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C151" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -3544,7 +3604,7 @@
         <v>153</v>
       </c>
       <c r="B152" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C152" t="s">
         <v>330</v>
@@ -3555,10 +3615,10 @@
         <v>154</v>
       </c>
       <c r="B153" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C153" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="154" spans="1:3">
@@ -3566,10 +3626,10 @@
         <v>155</v>
       </c>
       <c r="B154" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="C154" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -3577,7 +3637,7 @@
         <v>156</v>
       </c>
       <c r="B155" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="C155" t="s">
         <v>331</v>
@@ -3588,10 +3648,10 @@
         <v>157</v>
       </c>
       <c r="B156" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="C156" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="157" spans="1:3">
@@ -3599,10 +3659,10 @@
         <v>158</v>
       </c>
       <c r="B157" t="s">
-        <v>251</v>
+        <v>261</v>
       </c>
       <c r="C157" t="s">
-        <v>288</v>
+        <v>332</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -3610,10 +3670,10 @@
         <v>159</v>
       </c>
       <c r="B158" t="s">
-        <v>262</v>
+        <v>246</v>
       </c>
       <c r="C158" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -3621,10 +3681,10 @@
         <v>160</v>
       </c>
       <c r="B159" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C159" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="160" spans="1:3">
@@ -3632,10 +3692,10 @@
         <v>161</v>
       </c>
       <c r="B160" t="s">
-        <v>246</v>
+        <v>256</v>
       </c>
       <c r="C160" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="161" spans="1:3">
@@ -3643,7 +3703,7 @@
         <v>162</v>
       </c>
       <c r="B161" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="C161" t="s">
         <v>333</v>
@@ -3654,10 +3714,10 @@
         <v>163</v>
       </c>
       <c r="B162" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="C162" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -3665,10 +3725,10 @@
         <v>164</v>
       </c>
       <c r="B163" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C163" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="164" spans="1:3">
@@ -3679,7 +3739,7 @@
         <v>257</v>
       </c>
       <c r="C164" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -3687,10 +3747,10 @@
         <v>166</v>
       </c>
       <c r="B165" t="s">
-        <v>258</v>
+        <v>46</v>
       </c>
       <c r="C165" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="166" spans="1:3">
@@ -3698,10 +3758,10 @@
         <v>167</v>
       </c>
       <c r="B166" t="s">
-        <v>46</v>
+        <v>253</v>
       </c>
       <c r="C166" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -3709,10 +3769,10 @@
         <v>168</v>
       </c>
       <c r="B167" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="C167" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -3720,10 +3780,10 @@
         <v>169</v>
       </c>
       <c r="B168" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C168" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -3731,10 +3791,10 @@
         <v>170</v>
       </c>
       <c r="B169" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="C169" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -3742,10 +3802,10 @@
         <v>171</v>
       </c>
       <c r="B170" t="s">
-        <v>256</v>
+        <v>46</v>
       </c>
       <c r="C170" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="171" spans="1:3">
@@ -3753,10 +3813,10 @@
         <v>172</v>
       </c>
       <c r="B171" t="s">
-        <v>46</v>
+        <v>250</v>
       </c>
       <c r="C171" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -3764,10 +3824,10 @@
         <v>173</v>
       </c>
       <c r="B172" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="C172" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -3775,10 +3835,10 @@
         <v>174</v>
       </c>
       <c r="B173" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="C173" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="174" spans="1:3">
@@ -3797,7 +3857,7 @@
         <v>176</v>
       </c>
       <c r="B175" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C175" t="s">
         <v>336</v>
@@ -3808,10 +3868,10 @@
         <v>177</v>
       </c>
       <c r="B176" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="C176" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -3819,10 +3879,10 @@
         <v>178</v>
       </c>
       <c r="B177" t="s">
-        <v>246</v>
+        <v>257</v>
       </c>
       <c r="C177" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -3830,7 +3890,7 @@
         <v>179</v>
       </c>
       <c r="B178" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C178" t="s">
         <v>337</v>
@@ -3841,7 +3901,7 @@
         <v>180</v>
       </c>
       <c r="B179" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="C179" t="s">
         <v>337</v>
@@ -3852,10 +3912,10 @@
         <v>181</v>
       </c>
       <c r="B180" t="s">
-        <v>244</v>
+        <v>257</v>
       </c>
       <c r="C180" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="181" spans="1:3">
@@ -3863,7 +3923,7 @@
         <v>182</v>
       </c>
       <c r="B181" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C181" t="s">
         <v>338</v>
@@ -3874,7 +3934,7 @@
         <v>183</v>
       </c>
       <c r="B182" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="C182" t="s">
         <v>338</v>
@@ -3885,10 +3945,10 @@
         <v>184</v>
       </c>
       <c r="B183" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="C183" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="184" spans="1:3">
@@ -3896,10 +3956,10 @@
         <v>185</v>
       </c>
       <c r="B184" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C184" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="185" spans="1:3">
@@ -3907,7 +3967,7 @@
         <v>186</v>
       </c>
       <c r="B185" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="C185" t="s">
         <v>339</v>
@@ -3918,7 +3978,7 @@
         <v>187</v>
       </c>
       <c r="B186" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="C186" t="s">
         <v>339</v>
@@ -3929,10 +3989,10 @@
         <v>188</v>
       </c>
       <c r="B187" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C187" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="188" spans="1:3">
@@ -3940,10 +4000,10 @@
         <v>189</v>
       </c>
       <c r="B188" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="C188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="189" spans="1:3">
@@ -3951,10 +4011,10 @@
         <v>190</v>
       </c>
       <c r="B189" t="s">
-        <v>249</v>
+        <v>46</v>
       </c>
       <c r="C189" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="190" spans="1:3">
@@ -3962,10 +4022,10 @@
         <v>191</v>
       </c>
       <c r="B190" t="s">
-        <v>46</v>
+        <v>254</v>
       </c>
       <c r="C190" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -3973,10 +4033,10 @@
         <v>192</v>
       </c>
       <c r="B191" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="C191" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="192" spans="1:3">
@@ -3984,7 +4044,7 @@
         <v>193</v>
       </c>
       <c r="B192" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C192" t="s">
         <v>340</v>
@@ -3995,10 +4055,10 @@
         <v>194</v>
       </c>
       <c r="B193" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="C193" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="194" spans="1:3">
@@ -4006,10 +4066,10 @@
         <v>195</v>
       </c>
       <c r="B194" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="C194" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="195" spans="1:3">
@@ -4017,10 +4077,10 @@
         <v>196</v>
       </c>
       <c r="B195" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C195" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="196" spans="1:3">
@@ -4028,10 +4088,10 @@
         <v>197</v>
       </c>
       <c r="B196" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C196" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="197" spans="1:3">
@@ -4042,7 +4102,7 @@
         <v>253</v>
       </c>
       <c r="C197" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="198" spans="1:3">
@@ -4050,10 +4110,10 @@
         <v>199</v>
       </c>
       <c r="B198" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="C198" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="199" spans="1:3">
@@ -4061,7 +4121,7 @@
         <v>200</v>
       </c>
       <c r="B199" t="s">
-        <v>244</v>
+        <v>253</v>
       </c>
       <c r="C199" t="s">
         <v>342</v>
@@ -4072,10 +4132,10 @@
         <v>201</v>
       </c>
       <c r="B200" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C200" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="201" spans="1:3">
@@ -4083,7 +4143,7 @@
         <v>202</v>
       </c>
       <c r="B201" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C201" t="s">
         <v>343</v>
@@ -4094,10 +4154,10 @@
         <v>203</v>
       </c>
       <c r="B202" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C202" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="203" spans="1:3">
@@ -4105,10 +4165,10 @@
         <v>204</v>
       </c>
       <c r="B203" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="C203" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
     </row>
     <row r="204" spans="1:3">
@@ -4116,10 +4176,10 @@
         <v>205</v>
       </c>
       <c r="B204" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="C204" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
     </row>
     <row r="205" spans="1:3">
@@ -4127,10 +4187,10 @@
         <v>206</v>
       </c>
       <c r="B205" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="C205" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="206" spans="1:3">
@@ -4138,7 +4198,7 @@
         <v>207</v>
       </c>
       <c r="B206" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C206" t="s">
         <v>345</v>
@@ -4149,7 +4209,7 @@
         <v>208</v>
       </c>
       <c r="B207" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C207" t="s">
         <v>346</v>
@@ -4160,7 +4220,7 @@
         <v>209</v>
       </c>
       <c r="B208" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C208" t="s">
         <v>346</v>
@@ -4171,10 +4231,10 @@
         <v>210</v>
       </c>
       <c r="B209" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="C209" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="210" spans="1:3">
@@ -4182,10 +4242,10 @@
         <v>211</v>
       </c>
       <c r="B210" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
       <c r="C210" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="211" spans="1:3">
@@ -4193,7 +4253,7 @@
         <v>212</v>
       </c>
       <c r="B211" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="C211" t="s">
         <v>347</v>
@@ -4204,10 +4264,10 @@
         <v>213</v>
       </c>
       <c r="B212" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C212" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="213" spans="1:3">
@@ -4215,10 +4275,10 @@
         <v>214</v>
       </c>
       <c r="B213" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="C213" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="214" spans="1:3">
@@ -4226,10 +4286,10 @@
         <v>215</v>
       </c>
       <c r="B214" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
       <c r="C214" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="215" spans="1:3">
@@ -4237,10 +4297,10 @@
         <v>216</v>
       </c>
       <c r="B215" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C215" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
     </row>
     <row r="216" spans="1:3">
@@ -4248,10 +4308,10 @@
         <v>217</v>
       </c>
       <c r="B216" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="C216" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
     </row>
     <row r="217" spans="1:3">
@@ -4259,10 +4319,10 @@
         <v>218</v>
       </c>
       <c r="B217" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C217" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="218" spans="1:3">
@@ -4270,10 +4330,10 @@
         <v>219</v>
       </c>
       <c r="B218" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C218" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="219" spans="1:3">
@@ -4281,7 +4341,7 @@
         <v>220</v>
       </c>
       <c r="B219" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C219" t="s">
         <v>352</v>
@@ -4292,7 +4352,7 @@
         <v>221</v>
       </c>
       <c r="B220" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C220" t="s">
         <v>352</v>
@@ -4303,10 +4363,10 @@
         <v>222</v>
       </c>
       <c r="B221" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C221" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="222" spans="1:3">
@@ -4314,10 +4374,10 @@
         <v>223</v>
       </c>
       <c r="B222" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C222" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="223" spans="1:3">
@@ -4325,10 +4385,10 @@
         <v>224</v>
       </c>
       <c r="B223" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C223" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="224" spans="1:3">
@@ -4336,10 +4396,10 @@
         <v>225</v>
       </c>
       <c r="B224" t="s">
-        <v>251</v>
+        <v>261</v>
       </c>
       <c r="C224" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
     </row>
     <row r="225" spans="1:3">
@@ -4347,10 +4407,10 @@
         <v>226</v>
       </c>
       <c r="B225" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C225" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
     </row>
     <row r="226" spans="1:3">
@@ -4358,10 +4418,10 @@
         <v>227</v>
       </c>
       <c r="B226" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="C226" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
     </row>
     <row r="227" spans="1:3">
@@ -4369,10 +4429,10 @@
         <v>228</v>
       </c>
       <c r="B227" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C227" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="228" spans="1:3">
@@ -4380,7 +4440,7 @@
         <v>229</v>
       </c>
       <c r="B228" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C228" t="s">
         <v>356</v>
@@ -4391,7 +4451,7 @@
         <v>230</v>
       </c>
       <c r="B229" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="C229" t="s">
         <v>356</v>
@@ -4402,7 +4462,7 @@
         <v>231</v>
       </c>
       <c r="B230" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C230" t="s">
         <v>357</v>
@@ -4413,7 +4473,7 @@
         <v>232</v>
       </c>
       <c r="B231" t="s">
-        <v>244</v>
+        <v>257</v>
       </c>
       <c r="C231" t="s">
         <v>357</v>
@@ -4424,7 +4484,7 @@
         <v>233</v>
       </c>
       <c r="B232" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="C232" t="s">
         <v>357</v>
@@ -4435,7 +4495,7 @@
         <v>234</v>
       </c>
       <c r="B233" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="C233" t="s">
         <v>357</v>
@@ -4446,7 +4506,7 @@
         <v>235</v>
       </c>
       <c r="B234" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C234" t="s">
         <v>358</v>
@@ -4457,7 +4517,7 @@
         <v>236</v>
       </c>
       <c r="B235" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C235" t="s">
         <v>358</v>
@@ -4468,7 +4528,7 @@
         <v>237</v>
       </c>
       <c r="B236" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C236" t="s">
         <v>358</v>
@@ -4479,7 +4539,7 @@
         <v>238</v>
       </c>
       <c r="B237" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="C237" t="s">
         <v>358</v>
@@ -4490,10 +4550,10 @@
         <v>239</v>
       </c>
       <c r="B238" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="C238" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="239" spans="1:3">
@@ -4501,10 +4561,10 @@
         <v>240</v>
       </c>
       <c r="B239" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="C239" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="240" spans="1:3">
@@ -4512,10 +4572,10 @@
         <v>241</v>
       </c>
       <c r="B240" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="C240" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="241" spans="1:3">
@@ -4523,21 +4583,15 @@
         <v>242</v>
       </c>
       <c r="B241" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="C241" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="242" spans="1:3">
-      <c r="A242" t="s">
-        <v>243</v>
-      </c>
-      <c r="B242" t="s">
-        <v>258</v>
-      </c>
       <c r="C242" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -4547,7 +4601,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4555,562 +4609,650 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B2" t="s">
-        <v>403</v>
+        <v>412</v>
       </c>
       <c r="C2" t="s">
-        <v>433</v>
+        <v>443</v>
       </c>
       <c r="D2" t="s">
-        <v>468</v>
+        <v>482</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>365</v>
-      </c>
-      <c r="B3" t="s">
-        <v>404</v>
+        <v>366</v>
       </c>
       <c r="C3" t="s">
-        <v>434</v>
+        <v>444</v>
       </c>
       <c r="D3" t="s">
-        <v>469</v>
+        <v>483</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B4" t="s">
-        <v>405</v>
+        <v>413</v>
       </c>
       <c r="C4" t="s">
-        <v>435</v>
+        <v>445</v>
       </c>
       <c r="D4" t="s">
-        <v>470</v>
+        <v>484</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B5" t="s">
-        <v>406</v>
+        <v>414</v>
       </c>
       <c r="C5" t="s">
-        <v>436</v>
+        <v>446</v>
       </c>
       <c r="D5" t="s">
-        <v>471</v>
+        <v>485</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B6" t="s">
-        <v>407</v>
+        <v>415</v>
       </c>
       <c r="C6" t="s">
-        <v>437</v>
+        <v>447</v>
       </c>
       <c r="D6" t="s">
-        <v>472</v>
+        <v>486</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>369</v>
-      </c>
-      <c r="B7" t="s">
-        <v>404</v>
+        <v>370</v>
       </c>
       <c r="C7" t="s">
-        <v>438</v>
+        <v>448</v>
       </c>
       <c r="D7" t="s">
-        <v>473</v>
+        <v>487</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B8" t="s">
-        <v>408</v>
+        <v>416</v>
       </c>
       <c r="C8" t="s">
-        <v>439</v>
+        <v>449</v>
       </c>
       <c r="D8" t="s">
-        <v>474</v>
+        <v>488</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B9" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="C9" t="s">
-        <v>440</v>
+        <v>450</v>
       </c>
       <c r="D9" t="s">
-        <v>468</v>
+        <v>489</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B10" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="C10" t="s">
-        <v>441</v>
+        <v>451</v>
       </c>
       <c r="D10" t="s">
-        <v>475</v>
+        <v>490</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B11" t="s">
-        <v>407</v>
+        <v>418</v>
       </c>
       <c r="C11" t="s">
-        <v>442</v>
+        <v>452</v>
       </c>
       <c r="D11" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B12" t="s">
-        <v>411</v>
+        <v>419</v>
       </c>
       <c r="C12" t="s">
-        <v>443</v>
+        <v>453</v>
       </c>
       <c r="D12" t="s">
-        <v>477</v>
+        <v>491</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B13" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="C13" t="s">
-        <v>444</v>
+        <v>454</v>
       </c>
       <c r="D13" t="s">
-        <v>478</v>
+        <v>492</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B14" t="s">
-        <v>413</v>
+        <v>420</v>
       </c>
       <c r="C14" t="s">
-        <v>445</v>
+        <v>455</v>
       </c>
       <c r="D14" t="s">
-        <v>468</v>
+        <v>493</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>377</v>
-      </c>
-      <c r="B15" t="s">
-        <v>414</v>
+        <v>378</v>
       </c>
       <c r="C15" t="s">
-        <v>446</v>
+        <v>456</v>
       </c>
       <c r="D15" t="s">
-        <v>479</v>
+        <v>494</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B16" t="s">
-        <v>415</v>
+        <v>421</v>
       </c>
       <c r="C16" t="s">
-        <v>447</v>
+        <v>457</v>
       </c>
       <c r="D16" t="s">
-        <v>480</v>
+        <v>495</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B17" t="s">
-        <v>416</v>
+        <v>422</v>
       </c>
       <c r="C17" t="s">
-        <v>448</v>
+        <v>458</v>
       </c>
       <c r="D17" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B18" t="s">
-        <v>417</v>
+        <v>423</v>
       </c>
       <c r="C18" t="s">
-        <v>449</v>
+        <v>459</v>
       </c>
       <c r="D18" t="s">
-        <v>482</v>
+        <v>496</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B19" t="s">
-        <v>418</v>
+        <v>424</v>
       </c>
       <c r="C19" t="s">
-        <v>448</v>
+        <v>460</v>
       </c>
       <c r="D19" t="s">
-        <v>483</v>
+        <v>497</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B20" t="s">
-        <v>416</v>
+        <v>425</v>
       </c>
       <c r="C20" t="s">
-        <v>450</v>
+        <v>461</v>
       </c>
       <c r="D20" t="s">
-        <v>484</v>
+        <v>498</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B21" t="s">
-        <v>419</v>
+        <v>426</v>
       </c>
       <c r="C21" t="s">
-        <v>451</v>
+        <v>462</v>
       </c>
       <c r="D21" t="s">
-        <v>451</v>
+        <v>499</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>384</v>
-      </c>
-      <c r="B22" t="s">
-        <v>420</v>
+        <v>385</v>
       </c>
       <c r="C22" t="s">
-        <v>452</v>
+        <v>461</v>
       </c>
       <c r="D22" t="s">
-        <v>485</v>
+        <v>500</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B23" t="s">
-        <v>421</v>
+        <v>427</v>
       </c>
       <c r="C23" t="s">
-        <v>442</v>
+        <v>461</v>
       </c>
       <c r="D23" t="s">
-        <v>468</v>
+        <v>501</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>386</v>
-      </c>
-      <c r="B24" t="s">
-        <v>422</v>
+        <v>387</v>
       </c>
       <c r="C24" t="s">
-        <v>453</v>
+        <v>463</v>
       </c>
       <c r="D24" t="s">
-        <v>486</v>
+        <v>502</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B25" t="s">
-        <v>404</v>
+        <v>425</v>
       </c>
       <c r="C25" t="s">
-        <v>454</v>
+        <v>464</v>
       </c>
       <c r="D25" t="s">
-        <v>468</v>
+        <v>503</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B26" t="s">
-        <v>423</v>
+        <v>428</v>
       </c>
       <c r="C26" t="s">
-        <v>455</v>
+        <v>465</v>
       </c>
       <c r="D26" t="s">
-        <v>487</v>
+        <v>465</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B27" t="s">
-        <v>424</v>
+        <v>429</v>
       </c>
       <c r="C27" t="s">
-        <v>456</v>
+        <v>466</v>
       </c>
       <c r="D27" t="s">
-        <v>488</v>
+        <v>504</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B28" t="s">
-        <v>425</v>
+        <v>430</v>
       </c>
       <c r="C28" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="D28" t="s">
-        <v>489</v>
+        <v>482</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>391</v>
-      </c>
-      <c r="B29" t="s">
-        <v>426</v>
+        <v>392</v>
       </c>
       <c r="C29" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="D29" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B30" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="C30" t="s">
-        <v>459</v>
+        <v>467</v>
       </c>
       <c r="D30" t="s">
-        <v>491</v>
+        <v>505</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B31" t="s">
-        <v>407</v>
+        <v>422</v>
       </c>
       <c r="C31" t="s">
-        <v>460</v>
-      </c>
-      <c r="D31" t="s">
-        <v>492</v>
+        <v>462</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B32" t="s">
-        <v>428</v>
-      </c>
-      <c r="C32" t="s">
-        <v>461</v>
+        <v>432</v>
       </c>
       <c r="D32" t="s">
-        <v>468</v>
+        <v>506</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B33" t="s">
-        <v>429</v>
+        <v>413</v>
       </c>
       <c r="C33" t="s">
-        <v>462</v>
+        <v>468</v>
       </c>
       <c r="D33" t="s">
-        <v>493</v>
+        <v>482</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B34" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="C34" t="s">
-        <v>463</v>
+        <v>469</v>
       </c>
       <c r="D34" t="s">
-        <v>477</v>
+        <v>507</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B35" t="s">
-        <v>413</v>
+        <v>434</v>
       </c>
       <c r="C35" t="s">
-        <v>464</v>
+        <v>470</v>
       </c>
       <c r="D35" t="s">
-        <v>494</v>
+        <v>508</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B36" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="C36" t="s">
-        <v>465</v>
+        <v>471</v>
       </c>
       <c r="D36" t="s">
-        <v>495</v>
+        <v>509</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B37" t="s">
-        <v>418</v>
+        <v>436</v>
       </c>
       <c r="C37" t="s">
-        <v>466</v>
+        <v>472</v>
       </c>
       <c r="D37" t="s">
-        <v>496</v>
+        <v>510</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B38" t="s">
-        <v>416</v>
+        <v>437</v>
       </c>
       <c r="C38" t="s">
-        <v>448</v>
+        <v>473</v>
       </c>
       <c r="D38" t="s">
-        <v>497</v>
+        <v>511</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B39" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="C39" t="s">
-        <v>442</v>
+        <v>474</v>
       </c>
       <c r="D39" t="s">
-        <v>498</v>
+        <v>512</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B40" t="s">
-        <v>432</v>
+        <v>438</v>
       </c>
       <c r="C40" t="s">
-        <v>467</v>
+        <v>475</v>
       </c>
       <c r="D40" t="s">
-        <v>499</v>
+        <v>482</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>404</v>
+      </c>
+      <c r="B41" t="s">
+        <v>439</v>
+      </c>
+      <c r="C41" t="s">
+        <v>476</v>
+      </c>
+      <c r="D41" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>405</v>
+      </c>
+      <c r="B42" t="s">
+        <v>440</v>
+      </c>
+      <c r="C42" t="s">
+        <v>477</v>
+      </c>
+      <c r="D42" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>406</v>
+      </c>
+      <c r="B43" t="s">
+        <v>422</v>
+      </c>
+      <c r="C43" t="s">
+        <v>478</v>
+      </c>
+      <c r="D43" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>407</v>
+      </c>
+      <c r="B44" t="s">
+        <v>441</v>
+      </c>
+      <c r="C44" t="s">
+        <v>479</v>
+      </c>
+      <c r="D44" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>408</v>
+      </c>
+      <c r="B45" t="s">
+        <v>427</v>
+      </c>
+      <c r="C45" t="s">
+        <v>480</v>
+      </c>
+      <c r="D45" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>409</v>
+      </c>
+      <c r="B46" t="s">
+        <v>425</v>
+      </c>
+      <c r="C46" t="s">
+        <v>461</v>
+      </c>
+      <c r="D46" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>410</v>
+      </c>
+      <c r="B47" t="s">
+        <v>428</v>
+      </c>
+      <c r="C47" t="s">
+        <v>454</v>
+      </c>
+      <c r="D47" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>411</v>
+      </c>
+      <c r="B48" t="s">
+        <v>442</v>
+      </c>
+      <c r="C48" t="s">
+        <v>481</v>
+      </c>
+      <c r="D48" t="s">
+        <v>519</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updatated datasets, added ecosystems datasets
</commit_message>
<xml_diff>
--- a/data/download/Competences-Map-Dataset.xlsx
+++ b/data/download/Competences-Map-Dataset.xlsx
@@ -761,7 +761,7 @@
     <t>["A soup to remember", "Fabric Museum: TextLoom"]</t>
   </si>
   <si>
-    <t>["A soup to remember", "ARCHETIPI da Poseidonia a Paestum, ricerca di manufatti contemporanei", "MODAS: Sas Boghes da sos Singers a Tenor", "Polifonia Portal", "Synthetic Memories", "Swapmuseun", "Comuniterràe"]</t>
+    <t>["A soup to remember", "ARCHETIPI da Poseidonia a Paestum, ricerca di manufatti contemporanei", "MODAS: Sas Boghes da sos Singers a Tenor", "Polifonia Portal", "Synthetic Memories", "Swapmuseum", "Comuniterràe"]</t>
   </si>
   <si>
     <t>["A soup to remember", "Cultural Avatars", "Synthetic Memories"]</t>
@@ -779,7 +779,7 @@
     <t>["A soup to remember", "Pub Museums"]</t>
   </si>
   <si>
-    <t>["A soup to remember", "THE GREAT PALERMO", "Virtual Dance Museum", "TRACTION Opera co-creation for a social transformation", "Omni Chang’An Site Concept Show", "Synthetic Memories", "Craftal", "RISE UP - Revitalising Languages and Safeguarding Cultural Diversity", "Urban Media Archive, [unarchiving] program", "Swapmuseun", "MEMEX. MEMories and EXperiences for inclusive digital storytelling", "Quantum Temple Path to Alango", "Quantum Temple Passport"]</t>
+    <t>["A soup to remember", "THE GREAT PALERMO", "Virtual Dance Museum", "TRACTION Opera co-creation for a social transformation", "Omni Chang’An Site Concept Show", "Synthetic Memories", "Craftal", "RISE UP - Revitalising Languages and Safeguarding Cultural Diversity", "Urban Media Archive, [unarchiving] program", "Swapmuseum", "MEMEX. MEMories and EXperiences for inclusive digital storytelling", "Quantum Temple Path to Alango", "Quantum Temple Passport"]</t>
   </si>
   <si>
     <t>["A soup to remember", "Tempio del Brunello"]</t>
@@ -806,7 +806,7 @@
     <t>["Pub Museums", "Synthetic Memories", "Quantum Temple Path to Alango", "Quantum Temple Passport"]</t>
   </si>
   <si>
-    <t>["Pub Museums", "THE GREAT PALERMO", "Camino Al Mictlan NFT", "Whispering table", "Synthetic Memories", "Swapmuseun", "Comuniterràe", "Tacit Dialogues"]</t>
+    <t>["Pub Museums", "THE GREAT PALERMO", "Camino Al Mictlan NFT", "Whispering table", "Synthetic Memories", "Swapmuseum", "Comuniterràe", "Tacit Dialogues"]</t>
   </si>
   <si>
     <t>["THE GREAT PALERMO"]</t>
@@ -956,7 +956,7 @@
     <t>["Bamboo Weaving Mold"]</t>
   </si>
   <si>
-    <t>["Urban Media Archive, [unarchiving] program", "Swapmuseun"]</t>
+    <t>["Urban Media Archive, [unarchiving] program", "Swapmuseum"]</t>
   </si>
   <si>
     <t>["Urban Media Archive, [unarchiving] program"]</t>
@@ -968,7 +968,7 @@
     <t>["Urban Media Archive, [unarchiving] program", "Piccolo Museo del Diario"]</t>
   </si>
   <si>
-    <t>["Swapmuseun"]</t>
+    <t>["Swapmuseum"]</t>
   </si>
   <si>
     <t>["Comuniterràe"]</t>
@@ -1121,7 +1121,7 @@
     <t>Urban Media Archive, [unarchiving] program</t>
   </si>
   <si>
-    <t>Swapmuseun</t>
+    <t>Swapmuseum</t>
   </si>
   <si>
     <t>Comuniterràe</t>

</xml_diff>